<commit_message>
Alterações Gerais no Código
Alterações gerais para englobar a nova lógica
</commit_message>
<xml_diff>
--- a/SimuladorDeProcessador/ArquiteturaEp2.xlsx
+++ b/SimuladorDeProcessador/ArquiteturaEp2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Palavra de Controle</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>(INC)</t>
+  </si>
+  <si>
+    <t>Embora saibamos que o endereço é binário, utilizaremos ele inteiro para facilitar</t>
   </si>
 </sst>
 </file>
@@ -198,12 +201,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -216,15 +213,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -235,6 +227,21 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -243,10 +250,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2959,8 +2962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,104 +2985,104 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3"/>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="5" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="5"/>
+      <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="5"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="17"/>
       <c r="N4" s="3"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="15"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="8"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="15"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="D6" s="12"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
       <c r="N6" s="3"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="15"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5" t="s">
+      <c r="D7" s="12"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="5" t="s">
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="17" t="s">
         <v>2</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="15"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5"/>
+      <c r="D8" s="12"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="17"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -3087,13 +3090,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="15"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="10"/>
+      <c r="D9" s="12"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="8"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
@@ -3101,13 +3104,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="15"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="D10" s="12"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
@@ -3115,13 +3118,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="15"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="5" t="s">
+      <c r="D11" s="12"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="17" t="s">
         <v>3</v>
       </c>
       <c r="N11" s="3"/>
@@ -3131,13 +3134,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="15"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="5"/>
+      <c r="D12" s="12"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="17"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -3145,13 +3148,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="15"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="10"/>
+      <c r="D13" s="12"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="8"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
@@ -3159,13 +3162,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="15"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="8"/>
+      <c r="D14" s="12"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="6"/>
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
@@ -3173,13 +3176,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="15"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="5" t="s">
+      <c r="D15" s="12"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="17" t="s">
         <v>4</v>
       </c>
       <c r="N15" s="3"/>
@@ -3189,15 +3192,15 @@
         <v>12</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="15"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5" t="s">
+      <c r="D16" s="12"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="17"/>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -3205,13 +3208,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="15"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="10"/>
+      <c r="D17" s="12"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="8"/>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -3219,13 +3222,13 @@
         <v>14</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="15"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="D18" s="12"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -3233,13 +3236,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="15"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="5" t="s">
+      <c r="D19" s="12"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="17" t="s">
         <v>5</v>
       </c>
       <c r="N19" s="3"/>
@@ -3249,13 +3252,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="15"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="5"/>
+      <c r="D20" s="12"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="17"/>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -3263,13 +3266,13 @@
         <v>17</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="15"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="10"/>
+      <c r="D21" s="12"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="8"/>
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -3277,15 +3280,15 @@
         <v>18</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="15"/>
-      <c r="G22" s="5" t="s">
+      <c r="D22" s="12"/>
+      <c r="G22" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -3293,13 +3296,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="15"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="5" t="s">
+      <c r="D23" s="12"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="17" t="s">
         <v>6</v>
       </c>
       <c r="N23" s="3"/>
@@ -3309,13 +3312,13 @@
         <v>20</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="15"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="5"/>
+      <c r="D24" s="12"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="17"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -3323,13 +3326,13 @@
         <v>21</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="16"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="10"/>
+      <c r="D25" s="13"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="8"/>
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
@@ -3337,15 +3340,15 @@
         <v>22</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
@@ -3353,15 +3356,15 @@
         <v>23</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="18"/>
-      <c r="G27" s="5" t="s">
+      <c r="D27" s="20"/>
+      <c r="G27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="5" t="s">
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="17" t="s">
         <v>7</v>
       </c>
       <c r="N27" s="3"/>
@@ -3371,13 +3374,13 @@
         <v>24</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="18"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="5"/>
+      <c r="D28" s="20"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="17"/>
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -3385,7 +3388,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="18"/>
+      <c r="D29" s="20"/>
       <c r="J29" s="3"/>
       <c r="N29" s="3"/>
     </row>
@@ -3394,7 +3397,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="19"/>
+      <c r="D30" s="21"/>
       <c r="J30" s="3"/>
       <c r="N30" s="3"/>
     </row>
@@ -3403,281 +3406,287 @@
         <v>27</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J31" s="9"/>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>28</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="M32" s="4" t="s">
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="M32" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>29</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>30</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="15"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>31</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="13"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="16"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>32</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>33</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>34</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="15"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>35</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="12"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>36</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>37</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>38</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="12"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>39</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="12"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>40</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>41</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="15"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>42</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="15"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>43</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="15"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>44</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="15"/>
+      <c r="D48" s="12"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>45</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="15"/>
+      <c r="D49" s="12"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <v>46</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="15"/>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>47</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="15"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>48</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="15"/>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <v>49</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="15"/>
+      <c r="D53" s="12"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <v>50</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="15"/>
+      <c r="D54" s="12"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
         <v>51</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="15"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <v>52</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="15"/>
+      <c r="D56" s="12"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <v>53</v>
       </c>
       <c r="C57" s="1"/>
-      <c r="D57" s="15"/>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>54</v>
       </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="15"/>
+      <c r="D58" s="12"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
         <v>55</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="15"/>
+      <c r="D59" s="12"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>56</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="15"/>
+      <c r="D60" s="12"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>57</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="15"/>
+      <c r="D61" s="12"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>58</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="15"/>
+      <c r="D62" s="12"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>59</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="15"/>
+      <c r="D63" s="12"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>60</v>
       </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="15"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>61</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="15"/>
+      <c r="D65" s="12"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
         <v>62</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="15"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <v>63</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="16"/>
+      <c r="D67" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L23:L24"/>
     <mergeCell ref="D36:D67"/>
     <mergeCell ref="D33:D35"/>
     <mergeCell ref="P3:Q7"/>
@@ -3694,9 +3703,6 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L23:L24"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3714,12 +3720,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">

</xml_diff>

<commit_message>
Interpretação de Algumas instruções
Inclusão da interpretação de algumas instruções novas ao EP. INC, DEC,
ADD, SUB, MUL, DIV e MOV.
</commit_message>
<xml_diff>
--- a/SimuladorDeProcessador/ArquiteturaEp2.xlsx
+++ b/SimuladorDeProcessador/ArquiteturaEp2.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arquitetura" sheetId="1" r:id="rId1"/>
-    <sheet name="Mapa de Operações" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Mapa de Operações da ULA" sheetId="2" r:id="rId2"/>
+    <sheet name="Mapa de Controle de JUMP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Palavra de Controle</t>
   </si>
@@ -81,19 +81,85 @@
     <t>Controle de Jump</t>
   </si>
   <si>
-    <t>Endereço do Pulo (Conforme Especificação - &gt; Endereços de 32 bits</t>
-  </si>
-  <si>
     <t>00001</t>
   </si>
   <si>
-    <t>Adicionar 1</t>
-  </si>
-  <si>
-    <t>(INC)</t>
-  </si>
-  <si>
     <t>Embora saibamos que o endereço é binário, utilizaremos ele inteiro para facilitar</t>
+  </si>
+  <si>
+    <t>00010</t>
+  </si>
+  <si>
+    <t>00011</t>
+  </si>
+  <si>
+    <t>(INC _)</t>
+  </si>
+  <si>
+    <t>(DEC _)</t>
+  </si>
+  <si>
+    <t>Adicionar 1 ao registrador</t>
+  </si>
+  <si>
+    <t>Subtrair 1 ao registrador</t>
+  </si>
+  <si>
+    <t>Somar o valor do registrador 2 no registrador 1</t>
+  </si>
+  <si>
+    <t>(ADD 1, 2)</t>
+  </si>
+  <si>
+    <t>00100</t>
+  </si>
+  <si>
+    <t>Subtrair o valor do registrador 2 do registrador 1</t>
+  </si>
+  <si>
+    <t>(SUB 1, 2)</t>
+  </si>
+  <si>
+    <t>00101</t>
+  </si>
+  <si>
+    <t>(MUL _)</t>
+  </si>
+  <si>
+    <t>00111</t>
+  </si>
+  <si>
+    <t>Multiplicar o registrador A pelo registrador do operando e colocar o conteúdo no A</t>
+  </si>
+  <si>
+    <t>Dividir o conteúdo do registrador A pelo registrador do operando, e colocar o quociente no A e o resto no D</t>
+  </si>
+  <si>
+    <t>(DIV _)</t>
+  </si>
+  <si>
+    <t>Endereço do Pulo (Conforme Especificação - &gt; Endereços de 32 bits) OU ENTÃO DADO CONSTANTE PASSADO (EX: MOV)</t>
+  </si>
+  <si>
+    <t>Esse registrador ainda pode guardar uma constante passada (ex: MOV AX, 6)</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>Não faz nada</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento de dados</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento de endereço</t>
   </si>
 </sst>
 </file>
@@ -193,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -217,6 +283,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -235,9 +304,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -249,6 +315,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2962,8 +3031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,46 +3054,46 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3"/>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="11"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="17"/>
+      <c r="Q3" s="11"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="4"/>
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="17"/>
+      <c r="L4" s="11"/>
       <c r="N4" s="3"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="13"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="4"/>
@@ -3032,15 +3101,15 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="12"/>
+      <c r="D6" s="13"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -3048,41 +3117,41 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="N6" s="3"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="13"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="13"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="17"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="17"/>
+      <c r="L8" s="11"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -3090,7 +3159,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="13"/>
       <c r="G9" s="4"/>
       <c r="H9" s="8"/>
       <c r="I9" s="4"/>
@@ -3104,7 +3173,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="13"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3118,13 +3187,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="12"/>
+      <c r="D11" s="13"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="11" t="s">
         <v>3</v>
       </c>
       <c r="N11" s="3"/>
@@ -3134,13 +3203,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="12"/>
+      <c r="D12" s="13"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="17"/>
+      <c r="L12" s="11"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -3148,7 +3217,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="12"/>
+      <c r="D13" s="13"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -3162,7 +3231,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="12"/>
+      <c r="D14" s="13"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -3176,13 +3245,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="13"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="11" t="s">
         <v>4</v>
       </c>
       <c r="N15" s="3"/>
@@ -3192,15 +3261,15 @@
         <v>12</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="13"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="17"/>
+      <c r="L16" s="11"/>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -3208,9 +3277,9 @@
         <v>13</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="13"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
       <c r="K17" s="4"/>
@@ -3222,9 +3291,9 @@
         <v>14</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="13"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="17"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
@@ -3236,13 +3305,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="13"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="17" t="s">
+      <c r="L19" s="11" t="s">
         <v>5</v>
       </c>
       <c r="N19" s="3"/>
@@ -3252,13 +3321,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="12"/>
+      <c r="D20" s="13"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="17"/>
+      <c r="L20" s="11"/>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -3266,7 +3335,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="13"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -3280,11 +3349,11 @@
         <v>18</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="12"/>
-      <c r="G22" s="17" t="s">
+      <c r="D22" s="13"/>
+      <c r="G22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="4"/>
@@ -3296,13 +3365,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="12"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="D23" s="13"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="4"/>
       <c r="J23" s="5"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="17" t="s">
+      <c r="L23" s="11" t="s">
         <v>6</v>
       </c>
       <c r="N23" s="3"/>
@@ -3312,13 +3381,13 @@
         <v>20</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="12"/>
+      <c r="D24" s="13"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="17"/>
+      <c r="L24" s="11"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -3326,7 +3395,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="13"/>
+      <c r="D25" s="14"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -3357,14 +3426,14 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="20"/>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="5"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="17" t="s">
+      <c r="L27" s="11" t="s">
         <v>7</v>
       </c>
       <c r="N27" s="3"/>
@@ -3375,12 +3444,12 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="20"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="17"/>
+      <c r="L28" s="11"/>
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -3435,7 +3504,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3444,25 +3513,25 @@
         <v>30</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="15"/>
+      <c r="D34" s="16"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>31</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="16"/>
+      <c r="D35" s="17"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>32</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="11" t="s">
-        <v>21</v>
+      <c r="D36" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -3470,225 +3539,223 @@
         <v>33</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="12"/>
+      <c r="D37" s="20"/>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>34</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="12"/>
+      <c r="D38" s="20"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>35</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="12"/>
+      <c r="D39" s="20"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>36</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="12"/>
+      <c r="D40" s="20"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>37</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="12"/>
+      <c r="D41" s="20"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>38</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="12"/>
+      <c r="D42" s="20"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>39</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="12"/>
+      <c r="D43" s="20"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>40</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="12"/>
+      <c r="D44" s="20"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>41</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="12"/>
+      <c r="D45" s="20"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>42</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="12"/>
+      <c r="D46" s="20"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>43</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="12"/>
+      <c r="D47" s="20"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>44</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="12"/>
+      <c r="D48" s="20"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>45</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="12"/>
+      <c r="D49" s="20"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <v>46</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="12"/>
+      <c r="D50" s="20"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>47</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="12"/>
+      <c r="D51" s="20"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>48</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="12"/>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <v>49</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="12"/>
+      <c r="D53" s="20"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <v>50</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="12"/>
+      <c r="D54" s="20"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
         <v>51</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="12"/>
+      <c r="D55" s="20"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <v>52</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="12"/>
+      <c r="D56" s="20"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <v>53</v>
       </c>
       <c r="C57" s="1"/>
-      <c r="D57" s="12"/>
+      <c r="D57" s="20"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>54</v>
       </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="12"/>
+      <c r="D58" s="20"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
         <v>55</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="12"/>
+      <c r="D59" s="20"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>56</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="12"/>
+      <c r="D60" s="20"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>57</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="12"/>
+      <c r="D61" s="20"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>58</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="12"/>
+      <c r="D62" s="20"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>59</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="12"/>
+      <c r="D63" s="20"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>60</v>
       </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="12"/>
+      <c r="D64" s="20"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>61</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="12"/>
+      <c r="D65" s="20"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
         <v>62</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="12"/>
+      <c r="D66" s="20"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <v>63</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="13"/>
+      <c r="D67" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="D36:D67"/>
-    <mergeCell ref="D33:D35"/>
     <mergeCell ref="P3:Q7"/>
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="M32:O32"/>
@@ -3703,6 +3770,11 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="D36:D67"/>
+    <mergeCell ref="D33:D35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3712,27 +3784,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3742,12 +3870,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="96.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalização dos sinais e novas lógicas
Finalização da interpretação de sinais, alteração na lógica da memória.
</commit_message>
<xml_diff>
--- a/SimuladorDeProcessador/ArquiteturaEp2.xlsx
+++ b/SimuladorDeProcessador/ArquiteturaEp2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Arquitetura" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Palavra de Controle</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Sinais de Controle (Portas abertas)</t>
   </si>
   <si>
-    <t>Indicador de Operação</t>
-  </si>
-  <si>
     <t>Address Valid</t>
   </si>
   <si>
@@ -144,22 +141,103 @@
     <t>Esse registrador ainda pode guardar uma constante passada (ex: MOV AX, 6)</t>
   </si>
   <si>
-    <t>000</t>
-  </si>
-  <si>
     <t>Não faz nada</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento de dados</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
     <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento de endereço</t>
+  </si>
+  <si>
+    <t>Indicador de Operação da ULA</t>
+  </si>
+  <si>
+    <t>01000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtrair o valor do operando 2 do valor do operando 1 </t>
+  </si>
+  <si>
+    <t>(CMP 1, 2)</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>Instrução</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>JZ endereco</t>
+  </si>
+  <si>
+    <t>JMP endereco</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento somente se a Flag Zero estiver acesa</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>JNZ endereco</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento somente se a Flag Zero NÃO estiver acesa</t>
+  </si>
+  <si>
+    <t>JL endereco</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento somente se a flag zero estiver apagada E a flag de sinal estiver acesa</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento somente se a flag zero estiver apagada E a flag de sinal estiver apagada</t>
+  </si>
+  <si>
+    <t>JG endereco</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento somente se a flag zero estiver acesa OU a flag de sinal estiver acesa</t>
+  </si>
+  <si>
+    <t>JLE endereco</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está contido entre os bits 32 até 63 da palavra de controle no barramento somente se a flag zero estiver acesa OU a flag de sinal estiver apagada</t>
+  </si>
+  <si>
+    <t>JGE endereco</t>
+  </si>
+  <si>
+    <t>Coloca o valor que está no barramento de dado no barramento de endereço</t>
+  </si>
+  <si>
+    <t>1001</t>
   </si>
 </sst>
 </file>
@@ -175,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,8 +367,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -296,6 +386,15 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -304,20 +403,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3031,8 +3145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q67"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,46 +3168,46 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3"/>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="11"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="11"/>
+      <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
       <c r="I4" s="4"/>
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="11"/>
+      <c r="L4" s="12"/>
       <c r="N4" s="3"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="13"/>
+      <c r="D5" s="15"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="4"/>
@@ -3101,15 +3215,15 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="13"/>
+      <c r="D6" s="15"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -3117,41 +3231,41 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="N6" s="3"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="13"/>
+      <c r="D7" s="15"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="13"/>
+      <c r="D8" s="15"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="11"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="11"/>
+      <c r="L8" s="12"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -3159,7 +3273,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="13"/>
+      <c r="D9" s="15"/>
       <c r="G9" s="4"/>
       <c r="H9" s="8"/>
       <c r="I9" s="4"/>
@@ -3173,7 +3287,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="15"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3187,13 +3301,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="15"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="N11" s="3"/>
@@ -3203,13 +3317,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="15"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="11"/>
+      <c r="L12" s="12"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -3217,7 +3331,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="15"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -3231,7 +3345,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="15"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -3245,13 +3359,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="15"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="12" t="s">
         <v>4</v>
       </c>
       <c r="N15" s="3"/>
@@ -3261,15 +3375,15 @@
         <v>12</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="13"/>
+      <c r="D16" s="15"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="12" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="11"/>
+      <c r="L16" s="12"/>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -3277,9 +3391,9 @@
         <v>13</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="15"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="11"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
       <c r="K17" s="4"/>
@@ -3291,9 +3405,9 @@
         <v>14</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="15"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="11"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
@@ -3305,13 +3419,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="13"/>
+      <c r="D19" s="15"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="12" t="s">
         <v>5</v>
       </c>
       <c r="N19" s="3"/>
@@ -3321,13 +3435,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="15"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="11"/>
+      <c r="L20" s="12"/>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -3335,7 +3449,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="15"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -3349,11 +3463,11 @@
         <v>18</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="13"/>
-      <c r="G22" s="11" t="s">
+      <c r="D22" s="15"/>
+      <c r="G22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="11"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="4"/>
@@ -3365,13 +3479,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="13"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+      <c r="D23" s="15"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="4"/>
       <c r="J23" s="5"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="11" t="s">
+      <c r="L23" s="12" t="s">
         <v>6</v>
       </c>
       <c r="N23" s="3"/>
@@ -3381,13 +3495,13 @@
         <v>20</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="15"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="11"/>
+      <c r="L24" s="12"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -3395,7 +3509,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="14"/>
+      <c r="D25" s="16"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -3404,13 +3518,13 @@
       <c r="L25" s="8"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>22</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="19" t="s">
-        <v>17</v>
+      <c r="D26" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -3425,15 +3539,15 @@
         <v>23</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="20"/>
-      <c r="G27" s="11" t="s">
+      <c r="D27" s="18"/>
+      <c r="G27" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="5"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="11" t="s">
+      <c r="L27" s="12" t="s">
         <v>7</v>
       </c>
       <c r="N27" s="3"/>
@@ -3443,13 +3557,13 @@
         <v>24</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="20"/>
-      <c r="G28" s="11"/>
+      <c r="D28" s="18"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="11"/>
+      <c r="L28" s="12"/>
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -3457,7 +3571,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="18"/>
       <c r="J29" s="3"/>
       <c r="N29" s="3"/>
     </row>
@@ -3466,7 +3580,9 @@
         <v>26</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="21"/>
+      <c r="D30" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="J30" s="3"/>
       <c r="N30" s="3"/>
     </row>
@@ -3485,53 +3601,51 @@
         <v>28</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="18" t="s">
+      <c r="I32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="M32" s="18" t="s">
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="M32" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>29</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="D33" s="21"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>30</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="16"/>
+      <c r="D34" s="21"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>31</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="17"/>
+      <c r="D35" s="22"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>32</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="19" t="s">
-        <v>40</v>
+      <c r="D36" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -3539,9 +3653,9 @@
         <v>33</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="20"/>
+      <c r="D37" s="18"/>
       <c r="E37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -3549,218 +3663,221 @@
         <v>34</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="20"/>
+      <c r="D38" s="18"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>35</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="20"/>
+      <c r="D39" s="18"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>36</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="20"/>
+      <c r="D40" s="18"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>37</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="20"/>
+      <c r="D41" s="18"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>38</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="20"/>
+      <c r="D42" s="18"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>39</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="20"/>
+      <c r="D43" s="18"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>40</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="20"/>
+      <c r="D44" s="18"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>41</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="20"/>
+      <c r="D45" s="18"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>42</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="20"/>
+      <c r="D46" s="18"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>43</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="20"/>
+      <c r="D47" s="18"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>44</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="20"/>
+      <c r="D48" s="18"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>45</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="20"/>
+      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <v>46</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="20"/>
+      <c r="D50" s="18"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>47</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="20"/>
+      <c r="D51" s="18"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>48</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="20"/>
+      <c r="D52" s="18"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <v>49</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="20"/>
+      <c r="D53" s="18"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <v>50</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="20"/>
+      <c r="D54" s="18"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
         <v>51</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="20"/>
+      <c r="D55" s="18"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <v>52</v>
       </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="20"/>
+      <c r="D56" s="18"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <v>53</v>
       </c>
       <c r="C57" s="1"/>
-      <c r="D57" s="20"/>
+      <c r="D57" s="18"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>54</v>
       </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="20"/>
+      <c r="D58" s="18"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
         <v>55</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="20"/>
+      <c r="D59" s="18"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>56</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="20"/>
+      <c r="D60" s="18"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>57</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="20"/>
+      <c r="D61" s="18"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>58</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="20"/>
+      <c r="D62" s="18"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>59</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="20"/>
+      <c r="D63" s="18"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>60</v>
       </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="20"/>
+      <c r="D64" s="18"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>61</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="20"/>
+      <c r="D65" s="18"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
         <v>62</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="20"/>
+      <c r="D66" s="18"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <v>63</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="21"/>
+      <c r="D67" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="D36:D67"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D32:D35"/>
     <mergeCell ref="P3:Q7"/>
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="M32:O32"/>
     <mergeCell ref="D4:D25"/>
-    <mergeCell ref="D26:D30"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="G3:H4"/>
     <mergeCell ref="H7:H8"/>
@@ -3772,9 +3889,6 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="D36:D67"/>
-    <mergeCell ref="D33:D35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3784,83 +3898,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3870,41 +3995,138 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="96.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
+      <c r="C5" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>